<commit_message>
Updated Testing2 document after testing the test cases
</commit_message>
<xml_diff>
--- a/Testing/Testing 2.xlsx
+++ b/Testing/Testing 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganga\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aneesh Dalvi\Desktop\new_project\Breitenburg-SER515\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F0AB64E-2819-46CE-A6F1-8C28100FC1A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{447FC769-16B3-4FEC-88D4-A5AFDDF7CF29}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Related task #77</t>
+  </si>
+  <si>
+    <t>Aneesh Dalvi</t>
   </si>
 </sst>
 </file>
@@ -551,29 +554,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="8" max="8" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="90" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="93.75" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -599,7 +602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -609,8 +612,12 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
         <v>7</v>
@@ -619,7 +626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -629,8 +636,12 @@
       <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
@@ -641,7 +652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -651,8 +662,12 @@
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
@@ -663,7 +678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -673,8 +688,12 @@
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
@@ -685,7 +704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -695,8 +714,12 @@
       <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
@@ -707,7 +730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -717,8 +740,12 @@
       <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="F9" s="4" t="s">
         <v>27</v>
       </c>
@@ -741,7 +768,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -753,7 +780,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>